<commit_message>
New FAIRe NOAA checklist, version 2
</commit_message>
<xml_diff>
--- a/input/FAIRe_NOAA_checklist_v2.0.xlsx
+++ b/input/FAIRe_NOAA_checklist_v2.0.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29016"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayden.willms\Documents\Code\FAIReSheets\FAIReSheets\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4E7F94D-23DC-42DE-BBFC-EF498EB89520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F2115B1-91B3-4632-A170-4FD4F7FF0AC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1155" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4396" uniqueCount="1475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4374" uniqueCount="1468">
   <si>
     <t>Instructions for data submitters:</t>
   </si>
@@ -1614,7 +1614,7 @@
     <t>ampliconSize</t>
   </si>
   <si>
-    <t>The length of the amplicon in basepairs EXCLUDING the primers, adapters and MIDs. A range can be entered separated by a backslash "/" (i.e. 140/160). Unit = basepairs</t>
+    <t>The length of the amplicon in basepairs EXCLUDING the primers, adapters and MIDs. A range can be entered separated by a forward slash "/" (i.e. 140/160). Unit = basepairs</t>
   </si>
   <si>
     <t>basepairs</t>
@@ -4245,37 +4245,16 @@
     <t>The min_reads_cutoff was 1 read, but singletons were kept if the same sequence was detected in multiple samples. Data was curated using r-package LULU, minimum_mismatch cutoff 90%</t>
   </si>
   <si>
-    <t>output_read_count</t>
-  </si>
-  <si>
-    <t>The number of filtered sequence reads for each library (in an analysis), that made it through bioinforamtic filtering and used for final/subsequent analyses. Unit = reads</t>
-  </si>
-  <si>
-    <t>16847.0</t>
-  </si>
-  <si>
-    <t>https://w3id.org/nmdc/output_read_count</t>
-  </si>
-  <si>
-    <t>output_otu_num</t>
-  </si>
-  <si>
-    <t>Total number of OTUs or ASVs for each library (in an analysis)</t>
-  </si>
-  <si>
-    <t>86.0</t>
+    <t>otu_num_tax_assigned</t>
+  </si>
+  <si>
+    <t>Total number of OTUs or ASVs assigned to taxa based on the study-specific thresholds for each library (in an analysis)</t>
+  </si>
+  <si>
+    <t>49.0</t>
   </si>
   <si>
     <t>new</t>
-  </si>
-  <si>
-    <t>otu_num_tax_assigned</t>
-  </si>
-  <si>
-    <t>Total number of OTUs or ASVs assigned to taxa based on the study-specific thresholds for each library (in an analysis)</t>
-  </si>
-  <si>
-    <t>49.0</t>
   </si>
   <si>
     <t>discard_untrimmed</t>
@@ -5266,18 +5245,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R406"/>
+  <dimension ref="A1:R404"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I181" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="N189" sqref="N189"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C375" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="H376" sqref="H376"/>
       <selection pane="bottomLeft"/>
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="31.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
     <col min="3" max="3" width="26.42578125" customWidth="1"/>
     <col min="4" max="4" width="45.85546875" style="15" customWidth="1"/>
@@ -5292,6 +5271,7 @@
     <col min="13" max="13" width="29.85546875" style="15" customWidth="1"/>
     <col min="14" max="15" width="32.42578125" customWidth="1"/>
     <col min="16" max="16" width="58.28515625" customWidth="1"/>
+    <col min="17" max="17" width="49.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -18292,7 +18272,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="376" spans="1:18" ht="60.75">
+    <row r="376" spans="1:18" ht="45.75">
       <c r="A376" t="s">
         <v>1273</v>
       </c>
@@ -18314,20 +18294,14 @@
       <c r="H376" t="s">
         <v>306</v>
       </c>
-      <c r="I376" t="s">
-        <v>842</v>
-      </c>
       <c r="L376" s="15" t="s">
         <v>1393</v>
       </c>
       <c r="P376" t="s">
-        <v>130</v>
-      </c>
-      <c r="Q376" t="s">
+        <v>74</v>
+      </c>
+      <c r="R376" t="s">
         <v>1394</v>
-      </c>
-      <c r="R376" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="377" spans="1:18" ht="30.75">
@@ -18337,7 +18311,7 @@
       <c r="B377" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="C377" s="1" t="s">
+      <c r="C377" s="14" t="s">
         <v>1395</v>
       </c>
       <c r="D377" s="15" t="s">
@@ -18350,16 +18324,16 @@
         <v>68</v>
       </c>
       <c r="H377" t="s">
-        <v>306</v>
+        <v>115</v>
+      </c>
+      <c r="K377" t="s">
+        <v>116</v>
       </c>
       <c r="L377" s="15" t="s">
-        <v>1397</v>
+        <v>117</v>
       </c>
       <c r="P377" t="s">
-        <v>74</v>
-      </c>
-      <c r="R377" t="s">
-        <v>1398</v>
+        <v>165</v>
       </c>
     </row>
     <row r="378" spans="1:18" ht="45.75">
@@ -18369,11 +18343,11 @@
       <c r="B378" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="C378" s="1" t="s">
-        <v>1399</v>
+      <c r="C378" s="14" t="s">
+        <v>1397</v>
       </c>
       <c r="D378" s="15" t="s">
-        <v>1400</v>
+        <v>1398</v>
       </c>
       <c r="E378" s="12" t="s">
         <v>67</v>
@@ -18382,16 +18356,13 @@
         <v>68</v>
       </c>
       <c r="H378" t="s">
-        <v>306</v>
+        <v>60</v>
       </c>
       <c r="L378" s="15" t="s">
-        <v>1401</v>
+        <v>1399</v>
       </c>
       <c r="P378" t="s">
-        <v>74</v>
-      </c>
-      <c r="R378" t="s">
-        <v>1398</v>
+        <v>165</v>
       </c>
     </row>
     <row r="379" spans="1:18" ht="30.75">
@@ -18402,10 +18373,10 @@
         <v>1274</v>
       </c>
       <c r="C379" s="14" t="s">
-        <v>1402</v>
+        <v>1400</v>
       </c>
       <c r="D379" s="15" t="s">
-        <v>1403</v>
+        <v>1401</v>
       </c>
       <c r="E379" s="12" t="s">
         <v>67</v>
@@ -18414,19 +18385,19 @@
         <v>68</v>
       </c>
       <c r="H379" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K379" t="s">
-        <v>116</v>
+        <v>1402</v>
       </c>
       <c r="L379" s="15" t="s">
-        <v>117</v>
+        <v>1403</v>
       </c>
       <c r="P379" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="380" spans="1:18" ht="45.75">
+    <row r="380" spans="1:18" ht="106.5">
       <c r="A380" t="s">
         <v>1273</v>
       </c>
@@ -18445,17 +18416,24 @@
       <c r="F380" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="G380" t="s">
+        <v>1406</v>
+      </c>
       <c r="H380" t="s">
-        <v>60</v>
-      </c>
-      <c r="L380" s="15" t="s">
-        <v>1406</v>
+        <v>306</v>
+      </c>
+      <c r="I380" t="s">
+        <v>1293</v>
+      </c>
+      <c r="L380" s="15">
+        <v>220</v>
       </c>
       <c r="P380" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="381" spans="1:18" ht="30.75">
+      <c r="Q380" s="25"/>
+    </row>
+    <row r="381" spans="1:18" ht="106.5">
       <c r="A381" t="s">
         <v>1273</v>
       </c>
@@ -18474,14 +18452,17 @@
       <c r="F381" s="12" t="s">
         <v>68</v>
       </c>
+      <c r="G381" t="s">
+        <v>1409</v>
+      </c>
       <c r="H381" t="s">
-        <v>105</v>
-      </c>
-      <c r="K381" t="s">
-        <v>1409</v>
-      </c>
-      <c r="L381" s="15" t="s">
-        <v>1410</v>
+        <v>306</v>
+      </c>
+      <c r="I381" t="s">
+        <v>1293</v>
+      </c>
+      <c r="L381" s="15">
+        <v>220</v>
       </c>
       <c r="P381" t="s">
         <v>165</v>
@@ -18495,10 +18476,10 @@
         <v>1274</v>
       </c>
       <c r="C382" s="14" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D382" s="15" t="s">
         <v>1411</v>
-      </c>
-      <c r="D382" s="15" t="s">
-        <v>1412</v>
       </c>
       <c r="E382" s="12" t="s">
         <v>67</v>
@@ -18507,7 +18488,7 @@
         <v>68</v>
       </c>
       <c r="G382" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H382" t="s">
         <v>306</v>
@@ -18516,12 +18497,11 @@
         <v>1293</v>
       </c>
       <c r="L382" s="15">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="P382" t="s">
         <v>165</v>
       </c>
-      <c r="Q382" s="25"/>
     </row>
     <row r="383" spans="1:18" ht="106.5">
       <c r="A383" t="s">
@@ -18531,10 +18511,10 @@
         <v>1274</v>
       </c>
       <c r="C383" s="14" t="s">
-        <v>1414</v>
+        <v>1412</v>
       </c>
       <c r="D383" s="15" t="s">
-        <v>1415</v>
+        <v>1413</v>
       </c>
       <c r="E383" s="12" t="s">
         <v>67</v>
@@ -18543,7 +18523,7 @@
         <v>68</v>
       </c>
       <c r="G383" t="s">
-        <v>1416</v>
+        <v>1409</v>
       </c>
       <c r="H383" t="s">
         <v>306</v>
@@ -18552,13 +18532,13 @@
         <v>1293</v>
       </c>
       <c r="L383" s="15">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="P383" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="384" spans="1:18" ht="106.5">
+    <row r="384" spans="1:18" ht="76.5">
       <c r="A384" t="s">
         <v>1273</v>
       </c>
@@ -18566,10 +18546,10 @@
         <v>1274</v>
       </c>
       <c r="C384" s="14" t="s">
-        <v>1417</v>
+        <v>1414</v>
       </c>
       <c r="D384" s="15" t="s">
-        <v>1418</v>
+        <v>1415</v>
       </c>
       <c r="E384" s="12" t="s">
         <v>67</v>
@@ -18578,22 +18558,19 @@
         <v>68</v>
       </c>
       <c r="G384" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H384" t="s">
-        <v>306</v>
-      </c>
-      <c r="I384" t="s">
-        <v>1293</v>
-      </c>
-      <c r="L384" s="15">
-        <v>10</v>
+        <v>123</v>
+      </c>
+      <c r="L384" s="31">
+        <v>2</v>
       </c>
       <c r="P384" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="385" spans="1:16" ht="106.5">
+    <row r="385" spans="1:16" ht="91.5">
       <c r="A385" t="s">
         <v>1273</v>
       </c>
@@ -18601,10 +18578,10 @@
         <v>1274</v>
       </c>
       <c r="C385" s="14" t="s">
-        <v>1419</v>
+        <v>1416</v>
       </c>
       <c r="D385" s="15" t="s">
-        <v>1420</v>
+        <v>1417</v>
       </c>
       <c r="E385" s="12" t="s">
         <v>67</v>
@@ -18613,22 +18590,19 @@
         <v>68</v>
       </c>
       <c r="G385" t="s">
-        <v>1416</v>
+        <v>1409</v>
       </c>
       <c r="H385" t="s">
-        <v>306</v>
-      </c>
-      <c r="I385" t="s">
-        <v>1293</v>
-      </c>
-      <c r="L385" s="15">
-        <v>10</v>
+        <v>123</v>
+      </c>
+      <c r="L385" s="31">
+        <v>2</v>
       </c>
       <c r="P385" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="386" spans="1:16" ht="76.5">
+    <row r="386" spans="1:16" ht="121.5">
       <c r="A386" t="s">
         <v>1273</v>
       </c>
@@ -18636,10 +18610,10 @@
         <v>1274</v>
       </c>
       <c r="C386" s="14" t="s">
-        <v>1421</v>
+        <v>1418</v>
       </c>
       <c r="D386" s="15" t="s">
-        <v>1422</v>
+        <v>1419</v>
       </c>
       <c r="E386" s="12" t="s">
         <v>67</v>
@@ -18648,19 +18622,19 @@
         <v>68</v>
       </c>
       <c r="G386" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H386" t="s">
-        <v>123</v>
-      </c>
-      <c r="L386" s="31">
+        <v>306</v>
+      </c>
+      <c r="L386" s="15">
         <v>2</v>
       </c>
       <c r="P386" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="387" spans="1:16" ht="91.5">
+    <row r="387" spans="1:16" ht="76.5">
       <c r="A387" t="s">
         <v>1273</v>
       </c>
@@ -18668,10 +18642,10 @@
         <v>1274</v>
       </c>
       <c r="C387" s="14" t="s">
-        <v>1423</v>
+        <v>1420</v>
       </c>
       <c r="D387" s="15" t="s">
-        <v>1424</v>
+        <v>1421</v>
       </c>
       <c r="E387" s="12" t="s">
         <v>67</v>
@@ -18680,19 +18654,22 @@
         <v>68</v>
       </c>
       <c r="G387" t="s">
-        <v>1416</v>
+        <v>1406</v>
       </c>
       <c r="H387" t="s">
-        <v>123</v>
-      </c>
-      <c r="L387" s="31">
-        <v>2</v>
+        <v>105</v>
+      </c>
+      <c r="K387" t="s">
+        <v>1422</v>
+      </c>
+      <c r="L387" s="15" t="s">
+        <v>1423</v>
       </c>
       <c r="P387" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="388" spans="1:16" ht="121.5">
+    <row r="388" spans="1:16" ht="60.75">
       <c r="A388" t="s">
         <v>1273</v>
       </c>
@@ -18700,10 +18677,10 @@
         <v>1274</v>
       </c>
       <c r="C388" s="14" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D388" s="15" t="s">
         <v>1425</v>
-      </c>
-      <c r="D388" s="15" t="s">
-        <v>1426</v>
       </c>
       <c r="E388" s="12" t="s">
         <v>67</v>
@@ -18712,19 +18689,22 @@
         <v>68</v>
       </c>
       <c r="G388" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H388" t="s">
-        <v>306</v>
-      </c>
-      <c r="L388" s="15">
-        <v>2</v>
+        <v>105</v>
+      </c>
+      <c r="K388" s="26" t="s">
+        <v>1426</v>
+      </c>
+      <c r="L388" s="15" t="s">
+        <v>1427</v>
       </c>
       <c r="P388" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="389" spans="1:16" ht="76.5">
+    <row r="389" spans="1:16" ht="106.5">
       <c r="A389" t="s">
         <v>1273</v>
       </c>
@@ -18732,10 +18712,10 @@
         <v>1274</v>
       </c>
       <c r="C389" s="14" t="s">
-        <v>1427</v>
+        <v>1428</v>
       </c>
       <c r="D389" s="15" t="s">
-        <v>1428</v>
+        <v>1429</v>
       </c>
       <c r="E389" s="12" t="s">
         <v>67</v>
@@ -18744,16 +18724,13 @@
         <v>68</v>
       </c>
       <c r="G389" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H389" t="s">
-        <v>105</v>
-      </c>
-      <c r="K389" t="s">
-        <v>1429</v>
-      </c>
-      <c r="L389" s="15" t="s">
-        <v>1430</v>
+        <v>123</v>
+      </c>
+      <c r="L389" s="15">
+        <v>1</v>
       </c>
       <c r="P389" t="s">
         <v>165</v>
@@ -18767,10 +18744,10 @@
         <v>1274</v>
       </c>
       <c r="C390" s="14" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D390" s="15" t="s">
         <v>1431</v>
-      </c>
-      <c r="D390" s="15" t="s">
-        <v>1432</v>
       </c>
       <c r="E390" s="12" t="s">
         <v>67</v>
@@ -18779,22 +18756,19 @@
         <v>68</v>
       </c>
       <c r="G390" t="s">
-        <v>1413</v>
+        <v>1406</v>
       </c>
       <c r="H390" t="s">
-        <v>105</v>
-      </c>
-      <c r="K390" s="26" t="s">
-        <v>1433</v>
-      </c>
-      <c r="L390" s="15" t="s">
-        <v>1434</v>
+        <v>306</v>
+      </c>
+      <c r="L390" s="15">
+        <v>1000000</v>
       </c>
       <c r="P390" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="391" spans="1:16" ht="106.5">
+    <row r="391" spans="1:16">
       <c r="A391" t="s">
         <v>1273</v>
       </c>
@@ -18802,10 +18776,10 @@
         <v>1274</v>
       </c>
       <c r="C391" s="14" t="s">
-        <v>1435</v>
-      </c>
-      <c r="D391" s="15" t="s">
-        <v>1436</v>
+        <v>1432</v>
+      </c>
+      <c r="D391" t="s">
+        <v>1433</v>
       </c>
       <c r="E391" s="12" t="s">
         <v>67</v>
@@ -18814,19 +18788,19 @@
         <v>68</v>
       </c>
       <c r="G391" t="s">
-        <v>1413</v>
+        <v>1434</v>
       </c>
       <c r="H391" t="s">
-        <v>123</v>
+        <v>306</v>
       </c>
       <c r="L391" s="15">
-        <v>1</v>
+        <v>240</v>
       </c>
       <c r="P391" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="392" spans="1:16" ht="60.75">
+    <row r="392" spans="1:16">
       <c r="A392" t="s">
         <v>1273</v>
       </c>
@@ -18834,10 +18808,10 @@
         <v>1274</v>
       </c>
       <c r="C392" s="14" t="s">
-        <v>1437</v>
-      </c>
-      <c r="D392" s="15" t="s">
-        <v>1438</v>
+        <v>1435</v>
+      </c>
+      <c r="D392" t="s">
+        <v>1436</v>
       </c>
       <c r="E392" s="12" t="s">
         <v>67</v>
@@ -18846,13 +18820,13 @@
         <v>68</v>
       </c>
       <c r="G392" t="s">
-        <v>1413</v>
+        <v>1434</v>
       </c>
       <c r="H392" t="s">
-        <v>306</v>
+        <v>123</v>
       </c>
       <c r="L392" s="15">
-        <v>1000000</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="P392" t="s">
         <v>165</v>
@@ -18866,10 +18840,10 @@
         <v>1274</v>
       </c>
       <c r="C393" s="14" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D393" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="E393" s="12" t="s">
         <v>67</v>
@@ -18878,13 +18852,13 @@
         <v>68</v>
       </c>
       <c r="G393" t="s">
-        <v>1441</v>
+        <v>1434</v>
       </c>
       <c r="H393" t="s">
-        <v>306</v>
+        <v>123</v>
       </c>
       <c r="L393" s="15">
-        <v>240</v>
+        <v>0.01</v>
       </c>
       <c r="P393" t="s">
         <v>165</v>
@@ -18898,10 +18872,10 @@
         <v>1274</v>
       </c>
       <c r="C394" s="14" t="s">
-        <v>1442</v>
+        <v>1439</v>
       </c>
       <c r="D394" t="s">
-        <v>1443</v>
+        <v>1440</v>
       </c>
       <c r="E394" s="12" t="s">
         <v>67</v>
@@ -18910,13 +18884,13 @@
         <v>68</v>
       </c>
       <c r="G394" t="s">
-        <v>1441</v>
+        <v>1434</v>
       </c>
       <c r="H394" t="s">
-        <v>123</v>
+        <v>306</v>
       </c>
       <c r="L394" s="15">
-        <v>5.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="P394" t="s">
         <v>165</v>
@@ -18930,10 +18904,10 @@
         <v>1274</v>
       </c>
       <c r="C395" s="14" t="s">
-        <v>1444</v>
+        <v>1441</v>
       </c>
       <c r="D395" t="s">
-        <v>1445</v>
+        <v>1442</v>
       </c>
       <c r="E395" s="12" t="s">
         <v>67</v>
@@ -18942,13 +18916,13 @@
         <v>68</v>
       </c>
       <c r="G395" t="s">
-        <v>1441</v>
+        <v>1434</v>
       </c>
       <c r="H395" t="s">
-        <v>123</v>
+        <v>306</v>
       </c>
       <c r="L395" s="15">
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="P395" t="s">
         <v>165</v>
@@ -18962,10 +18936,10 @@
         <v>1274</v>
       </c>
       <c r="C396" s="14" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="D396" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
       <c r="E396" s="12" t="s">
         <v>67</v>
@@ -18974,19 +18948,19 @@
         <v>68</v>
       </c>
       <c r="G396" t="s">
-        <v>1441</v>
+        <v>1434</v>
       </c>
       <c r="H396" t="s">
         <v>306</v>
       </c>
       <c r="L396" s="15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P396" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="397" spans="1:16">
+    <row r="397" spans="1:16" ht="121.5">
       <c r="A397" t="s">
         <v>1273</v>
       </c>
@@ -18994,31 +18968,28 @@
         <v>1274</v>
       </c>
       <c r="C397" s="14" t="s">
-        <v>1448</v>
-      </c>
-      <c r="D397" t="s">
-        <v>1449</v>
-      </c>
-      <c r="E397" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F397" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G397" t="s">
-        <v>1441</v>
+        <v>1445</v>
+      </c>
+      <c r="D397" s="15" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E397" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F397" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="H397" t="s">
-        <v>306</v>
+        <v>123</v>
       </c>
       <c r="L397" s="15">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="P397" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="398" spans="1:16">
+    <row r="398" spans="1:16" ht="60.75">
       <c r="A398" t="s">
         <v>1273</v>
       </c>
@@ -19026,31 +18997,31 @@
         <v>1274</v>
       </c>
       <c r="C398" s="14" t="s">
-        <v>1450</v>
-      </c>
-      <c r="D398" t="s">
-        <v>1451</v>
-      </c>
-      <c r="E398" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F398" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G398" t="s">
-        <v>1441</v>
+        <v>1447</v>
+      </c>
+      <c r="D398" s="15" t="s">
+        <v>1448</v>
+      </c>
+      <c r="E398" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F398" s="27" t="s">
+        <v>98</v>
       </c>
       <c r="H398" t="s">
         <v>306</v>
       </c>
+      <c r="I398" t="s">
+        <v>1449</v>
+      </c>
       <c r="L398" s="15">
-        <v>2</v>
+        <v>250</v>
       </c>
       <c r="P398" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="399" spans="1:16" ht="121.5">
+    <row r="399" spans="1:16" ht="60.75">
       <c r="A399" t="s">
         <v>1273</v>
       </c>
@@ -19058,10 +19029,10 @@
         <v>1274</v>
       </c>
       <c r="C399" s="14" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="D399" s="15" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="E399" s="27" t="s">
         <v>97</v>
@@ -19070,16 +19041,19 @@
         <v>98</v>
       </c>
       <c r="H399" t="s">
-        <v>123</v>
+        <v>306</v>
+      </c>
+      <c r="I399" t="s">
+        <v>1449</v>
       </c>
       <c r="L399" s="15">
-        <v>0.01</v>
+        <v>100</v>
       </c>
       <c r="P399" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="400" spans="1:16" ht="60.75">
+    <row r="400" spans="1:16" ht="106.5">
       <c r="A400" t="s">
         <v>1273</v>
       </c>
@@ -19087,10 +19061,10 @@
         <v>1274</v>
       </c>
       <c r="C400" s="14" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="D400" s="15" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="E400" s="27" t="s">
         <v>97</v>
@@ -19099,19 +19073,16 @@
         <v>98</v>
       </c>
       <c r="H400" t="s">
-        <v>306</v>
-      </c>
-      <c r="I400" t="s">
-        <v>1456</v>
+        <v>123</v>
       </c>
       <c r="L400" s="15">
-        <v>250</v>
+        <v>0.01</v>
       </c>
       <c r="P400" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="401" spans="1:16" ht="60.75">
+    <row r="401" spans="1:16" ht="76.5">
       <c r="A401" t="s">
         <v>1273</v>
       </c>
@@ -19119,31 +19090,31 @@
         <v>1274</v>
       </c>
       <c r="C401" s="14" t="s">
-        <v>1457</v>
+        <v>1454</v>
       </c>
       <c r="D401" s="15" t="s">
-        <v>1458</v>
-      </c>
-      <c r="E401" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F401" s="27" t="s">
-        <v>98</v>
+        <v>1455</v>
+      </c>
+      <c r="E401" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F401" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G401" t="s">
+        <v>1456</v>
       </c>
       <c r="H401" t="s">
-        <v>306</v>
-      </c>
-      <c r="I401" t="s">
-        <v>1456</v>
+        <v>123</v>
       </c>
       <c r="L401" s="15">
-        <v>100</v>
+        <v>0.8</v>
       </c>
       <c r="P401" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="402" spans="1:16" ht="106.5">
+    <row r="402" spans="1:16" ht="121.5">
       <c r="A402" t="s">
         <v>1273</v>
       </c>
@@ -19151,147 +19122,86 @@
         <v>1274</v>
       </c>
       <c r="C402" s="14" t="s">
+        <v>1457</v>
+      </c>
+      <c r="D402" s="15" t="s">
+        <v>1458</v>
+      </c>
+      <c r="E402" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F402" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="G402" t="s">
         <v>1459</v>
-      </c>
-      <c r="D402" s="15" t="s">
-        <v>1460</v>
-      </c>
-      <c r="E402" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="F402" s="27" t="s">
-        <v>98</v>
-      </c>
-      <c r="H402" t="s">
-        <v>123</v>
-      </c>
-      <c r="L402" s="15">
-        <v>0.01</v>
       </c>
       <c r="P402" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="403" spans="1:16" ht="76.5">
+    <row r="403" spans="1:16" ht="30.75">
       <c r="A403" t="s">
         <v>1273</v>
       </c>
-      <c r="B403" s="5" t="s">
+      <c r="B403" s="28" t="s">
         <v>1274</v>
       </c>
       <c r="C403" s="14" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D403" s="15" t="s">
         <v>1461</v>
       </c>
-      <c r="D403" s="15" t="s">
+      <c r="E403" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F403" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="H403" t="s">
+        <v>105</v>
+      </c>
+      <c r="K403" t="s">
         <v>1462</v>
       </c>
-      <c r="E403" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F403" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G403" t="s">
+      <c r="L403" s="15" t="s">
         <v>1463</v>
       </c>
-      <c r="H403" t="s">
-        <v>123</v>
-      </c>
-      <c r="L403" s="15">
-        <v>0.8</v>
-      </c>
       <c r="P403" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="404" spans="1:16" ht="121.5">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="404" spans="1:16" ht="45.75">
       <c r="A404" t="s">
         <v>1273</v>
       </c>
-      <c r="B404" s="5" t="s">
+      <c r="B404" s="28" t="s">
         <v>1274</v>
       </c>
       <c r="C404" s="14" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D404" s="15" t="s">
+        <v>1466</v>
+      </c>
+      <c r="E404" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="F404" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G404" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H404" t="s">
+        <v>123</v>
+      </c>
+      <c r="L404" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="P404" t="s">
         <v>1464</v>
-      </c>
-      <c r="D404" s="15" t="s">
-        <v>1465</v>
-      </c>
-      <c r="E404" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F404" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G404" t="s">
-        <v>1466</v>
-      </c>
-      <c r="P404" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="405" spans="1:16" ht="30.75">
-      <c r="A405" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B405" s="28" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C405" s="14" t="s">
-        <v>1467</v>
-      </c>
-      <c r="D405" s="15" t="s">
-        <v>1468</v>
-      </c>
-      <c r="E405" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F405" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="H405" t="s">
-        <v>105</v>
-      </c>
-      <c r="K405" t="s">
-        <v>1469</v>
-      </c>
-      <c r="L405" s="15" t="s">
-        <v>1470</v>
-      </c>
-      <c r="P405" t="s">
-        <v>1471</v>
-      </c>
-    </row>
-    <row r="406" spans="1:16" ht="45.75">
-      <c r="A406" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B406" s="28" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C406" s="14" t="s">
-        <v>1472</v>
-      </c>
-      <c r="D406" s="15" t="s">
-        <v>1473</v>
-      </c>
-      <c r="E406" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="F406" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="G406" t="s">
-        <v>1474</v>
-      </c>
-      <c r="H406" t="s">
-        <v>123</v>
-      </c>
-      <c r="L406" s="15">
-        <v>0.8</v>
-      </c>
-      <c r="P406" t="s">
-        <v>1471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>